<commit_message>
fixed the error of invalid token and other changes
</commit_message>
<xml_diff>
--- a/server/dispatch_report.xlsx
+++ b/server/dispatch_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>sr No.</t>
   </si>
@@ -46,34 +46,46 @@
     <t>D001</t>
   </si>
   <si>
+    <t>T001</t>
+  </si>
+  <si>
+    <t>MH04DE1433</t>
+  </si>
+  <si>
+    <t>2020-04-15</t>
+  </si>
+  <si>
+    <t>S006</t>
+  </si>
+  <si>
+    <t>D005</t>
+  </si>
+  <si>
     <t>T002</t>
   </si>
   <si>
-    <t>MH04AB1234</t>
-  </si>
-  <si>
-    <t>2020-05-03</t>
-  </si>
-  <si>
-    <t>S005</t>
+    <t>mh05fr3434</t>
+  </si>
+  <si>
+    <t>2020-04-16</t>
   </si>
   <si>
     <t>D002</t>
   </si>
   <si>
-    <t>T003</t>
-  </si>
-  <si>
-    <t>MH04-AB-1234</t>
-  </si>
-  <si>
-    <t>2020-01-10</t>
-  </si>
-  <si>
-    <t>04AB1234</t>
-  </si>
-  <si>
-    <t>MHAB12</t>
+    <t>mh462390</t>
+  </si>
+  <si>
+    <t>2020-02-11</t>
+  </si>
+  <si>
+    <t>mh083567</t>
+  </si>
+  <si>
+    <t>2020-04-18</t>
+  </si>
+  <si>
+    <t>2020-02-18</t>
   </si>
 </sst>
 </file>
@@ -445,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -471,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -497,25 +509,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15">
@@ -523,25 +535,25 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15">
@@ -549,25 +561,25 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>